<commit_message>
Running Model on CaseA December 4th
</commit_message>
<xml_diff>
--- a/test files/Scoring_Sheet_Test_Files_Team_6_December4th.xlsx
+++ b/test files/Scoring_Sheet_Test_Files_Team_6_December4th.xlsx
@@ -5232,7 +5232,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
@@ -5802,116 +5804,104 @@
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
       <c r="D16" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E16" s="4">
-        <f t="shared" ref="E16:E22" si="4">1/24</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F16" s="4">
-        <f t="shared" ref="F15:P22" si="5">1/24</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G16" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="H16" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I16" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J16" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.01</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.01</v>
       </c>
       <c r="K16" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L16" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.21614</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0.01</v>
       </c>
       <c r="M16" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.10412425</v>
       </c>
       <c r="N16" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.15030487000000001</v>
       </c>
       <c r="O16" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.21260486000000001</v>
       </c>
       <c r="P16" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.23682601</v>
       </c>
       <c r="R16" s="3">
         <f t="shared" si="2"/>
-        <v>0.99999999999999956</v>
+        <v>0.99999999000000006</v>
       </c>
       <c r="T16" s="11">
-        <f t="shared" ref="T16:T22" si="6">SUM(V16:AH16)</f>
-        <v>0</v>
+        <f t="shared" ref="T16:T22" si="4">SUM(V16:AH16)</f>
+        <v>2.5068619430393726</v>
       </c>
       <c r="U16" s="13"/>
       <c r="V16">
-        <f t="shared" ref="V16:AH22" si="7">LOG(D16/D$3, 2)*D$24</f>
+        <f t="shared" ref="V16:AH22" si="5">LOG(D16/D$3, 2)*D$24</f>
         <v>0</v>
       </c>
       <c r="W16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AC16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AD16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AE16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AF16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AG16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AH16">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2.5068619430393726</v>
       </c>
     </row>
     <row r="17" spans="1:34" ht="18.75">
@@ -5921,116 +5911,104 @@
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
       <c r="D17" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E17" s="4">
-        <f t="shared" si="4"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F17" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G17" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="H17" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I17" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J17" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="K17" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.01</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.01</v>
       </c>
       <c r="L17" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.14315918</v>
       </c>
       <c r="M17" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>3.4034420000000003E-2</v>
       </c>
       <c r="N17" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>8.0970020000000004E-2</v>
       </c>
       <c r="O17" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.43090110999999998</v>
       </c>
       <c r="P17" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.23093527999999999</v>
       </c>
       <c r="R17" s="3">
         <f t="shared" si="2"/>
-        <v>0.99999999999999956</v>
+        <v>1.0000000099999999</v>
       </c>
       <c r="T17" s="11">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>2.4705229964121602</v>
       </c>
       <c r="U17" s="13"/>
       <c r="V17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AC17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AD17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AE17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AF17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AG17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AH17">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2.4705229964121602</v>
       </c>
     </row>
     <row r="18" spans="1:34" ht="18.75">
@@ -6040,116 +6018,104 @@
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
       <c r="D18" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E18" s="4">
-        <f t="shared" si="4"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F18" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G18" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="H18" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I18" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J18" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.01</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0.01</v>
       </c>
       <c r="K18" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L18" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.2610100000000001E-2</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0.01</v>
       </c>
       <c r="M18" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.20161196000000001</v>
       </c>
       <c r="N18" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.30504652999999998</v>
       </c>
       <c r="O18" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.17380933000000001</v>
       </c>
       <c r="P18" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.22692208</v>
       </c>
       <c r="R18" s="3">
         <f t="shared" si="2"/>
-        <v>0.99999999999999956</v>
+        <v>1</v>
       </c>
       <c r="T18" s="11">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>2.4452313989634242</v>
       </c>
       <c r="U18" s="13"/>
       <c r="V18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AC18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AD18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AE18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AF18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AG18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AH18">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2.4452313989634242</v>
       </c>
     </row>
     <row r="19" spans="1:34" ht="18.75">
@@ -6176,60 +6142,60 @@
         <v>0</v>
       </c>
       <c r="T19" s="11" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
       <c r="U19" s="13"/>
       <c r="V19" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="W19" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="X19" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="Y19" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="Z19" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AA19" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AB19" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AC19" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AD19" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AE19" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AF19" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AG19" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AH19" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -6257,60 +6223,60 @@
         <v>0</v>
       </c>
       <c r="T20" s="11" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
       <c r="U20" s="13"/>
       <c r="V20" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="W20" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="X20" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="Y20" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="Z20" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AA20" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AB20" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AC20" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AD20" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AE20" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AF20" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AG20" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AH20" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -6338,60 +6304,60 @@
         <v>0</v>
       </c>
       <c r="T21" s="11" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
       <c r="U21" s="13"/>
       <c r="V21" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="W21" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="X21" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="Y21" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="Z21" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AA21" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AB21" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AC21" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AD21" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AE21" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AF21" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AG21" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AH21" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -6419,60 +6385,60 @@
         <v>0</v>
       </c>
       <c r="T22" s="11" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
       <c r="U22" s="13"/>
       <c r="V22" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="W22" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="X22" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="Y22" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="Z22" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AA22" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AB22" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AC22" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AD22" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AE22" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AF22" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AG22" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="AH22" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -6556,51 +6522,51 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" ref="F26:P33" si="8">1/24</f>
+        <f t="shared" ref="F26:P29" si="6">1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R26" s="3">
-        <f t="shared" ref="R26:R33" si="9">SUM(D26:P26)</f>
+        <f t="shared" ref="R26:R33" si="7">SUM(D26:P26)</f>
         <v>0.99999999999999956</v>
       </c>
       <c r="T26" s="11">
@@ -6613,51 +6579,51 @@
         <v>0</v>
       </c>
       <c r="W26">
-        <f t="shared" ref="W26:AH33" si="10">LOG(E26/E$3, 2)*E$35</f>
+        <f t="shared" ref="W26:AH33" si="8">LOG(E26/E$3, 2)*E$35</f>
         <v>0</v>
       </c>
       <c r="X26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Y26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AA26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AB26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AF26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AG26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -6675,108 +6641,108 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F27" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J27" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K27" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L27" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M27" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N27" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O27" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P27" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R27" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T27" s="11">
-        <f t="shared" ref="T27:T33" si="11">SUM(V27:AH27)</f>
+        <f t="shared" ref="T27:T33" si="9">SUM(V27:AH27)</f>
         <v>0</v>
       </c>
       <c r="U27" s="13"/>
       <c r="V27">
-        <f t="shared" ref="V27:V33" si="12">LOG(D27/D$3, 2)*D$35</f>
+        <f t="shared" ref="V27:V33" si="10">LOG(D27/D$3, 2)*D$35</f>
         <v>0</v>
       </c>
       <c r="W27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AA27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AB27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AF27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AG27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -6790,112 +6756,112 @@
         <v>0.5</v>
       </c>
       <c r="E28" s="4">
-        <f t="shared" ref="E28:E33" si="13">1/24</f>
+        <f t="shared" ref="E28:E29" si="11">1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F28" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G28" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H28" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I28" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J28" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K28" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L28" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M28" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N28" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O28" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P28" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R28" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T28" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U28" s="13"/>
       <c r="V28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="W28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Y28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AA28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AB28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AF28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AG28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -6909,112 +6875,112 @@
         <v>0.5</v>
       </c>
       <c r="E29" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F29" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G29" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I29" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J29" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K29" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L29" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M29" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N29" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O29" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P29" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R29" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T29" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U29" s="13"/>
       <c r="V29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="W29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Y29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AA29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AB29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AF29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AG29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -7038,64 +7004,64 @@
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="R30" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T30" s="11" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>#NUM!</v>
       </c>
       <c r="U30" s="13"/>
       <c r="V30" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>#NUM!</v>
       </c>
       <c r="W30" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="X30" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="Y30" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="Z30" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AA30" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AB30" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AC30" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AD30" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AE30" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AF30" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AG30" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AH30" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -7119,64 +7085,64 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="R31" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T31" s="11" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>#NUM!</v>
       </c>
       <c r="U31" s="13"/>
       <c r="V31" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>#NUM!</v>
       </c>
       <c r="W31" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="X31" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="Y31" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="Z31" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AA31" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AB31" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AC31" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AD31" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AE31" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AF31" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AG31" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AH31" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -7200,64 +7166,64 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="R32" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T32" s="11" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>#NUM!</v>
       </c>
       <c r="U32" s="13"/>
       <c r="V32" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>#NUM!</v>
       </c>
       <c r="W32" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="X32" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="Y32" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="Z32" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AA32" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AB32" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AC32" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AD32" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AE32" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AF32" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AG32" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AH32" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -7281,60 +7247,60 @@
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="R33" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T33" s="11" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>#NUM!</v>
       </c>
       <c r="U33" s="13"/>
       <c r="V33" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>#NUM!</v>
       </c>
       <c r="W33" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="X33" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="Y33" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="Z33" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AA33" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AB33" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AC33" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AD33" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AE33" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AF33" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AG33" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
       <c r="AH33" t="e">
@@ -7433,51 +7399,51 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F37" s="4">
-        <f t="shared" ref="F37:P44" si="14">1/24</f>
+        <f t="shared" ref="F37:P40" si="12">1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G37" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H37" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I37" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J37" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K37" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L37" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M37" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N37" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O37" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P37" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R37" s="3">
-        <f t="shared" ref="R37:R44" si="15">SUM(D37:P37)</f>
+        <f t="shared" ref="R37:R44" si="13">SUM(D37:P37)</f>
         <v>0.99999999999999956</v>
       </c>
       <c r="T37" s="11">
@@ -7490,51 +7456,51 @@
         <v>0</v>
       </c>
       <c r="W37">
-        <f t="shared" ref="W37:AH44" si="16">LOG(E37/E$3, 2)*E$46</f>
+        <f t="shared" ref="W37:AH44" si="14">LOG(E37/E$3, 2)*E$46</f>
         <v>0</v>
       </c>
       <c r="X37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Z37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AA37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AB37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AC37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AD37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AE37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AF37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AG37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -7548,112 +7514,112 @@
         <v>0.5</v>
       </c>
       <c r="E38" s="4">
-        <f t="shared" ref="E38:E44" si="17">1/24</f>
+        <f t="shared" ref="E38:E40" si="15">1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F38" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G38" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H38" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I38" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J38" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K38" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L38" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M38" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N38" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O38" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P38" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R38" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T38" s="11">
-        <f t="shared" ref="T38:T44" si="18">SUM(V38:AH38)</f>
+        <f t="shared" ref="T38:T44" si="16">SUM(V38:AH38)</f>
         <v>0</v>
       </c>
       <c r="U38" s="13"/>
       <c r="V38">
-        <f t="shared" ref="V38:V44" si="19">LOG(D38/D$3, 2)*D$46</f>
+        <f t="shared" ref="V38:V44" si="17">LOG(D38/D$3, 2)*D$46</f>
         <v>0</v>
       </c>
       <c r="W38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Z38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AA38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AB38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AC38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AD38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AE38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AF38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AG38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -7667,112 +7633,112 @@
         <v>0.5</v>
       </c>
       <c r="E39" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F39" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G39" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H39" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I39" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J39" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K39" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L39" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M39" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N39" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O39" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P39" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R39" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T39" s="11">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U39" s="13"/>
       <c r="V39">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="W39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Z39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AA39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AB39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AC39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AD39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AE39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AF39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AG39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -7786,112 +7752,112 @@
         <v>0.5</v>
       </c>
       <c r="E40" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F40" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G40" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H40" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I40" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J40" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K40" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L40" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M40" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N40" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O40" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P40" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R40" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T40" s="11">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U40" s="13"/>
       <c r="V40">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="W40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Z40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AA40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AB40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AC40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AD40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AE40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AF40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AG40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -7915,64 +7881,64 @@
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
       <c r="R41" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T41" s="11" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
       <c r="U41" s="13"/>
       <c r="V41" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>#NUM!</v>
       </c>
       <c r="W41" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="X41" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="Y41" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="Z41" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AA41" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AB41" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AC41" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AD41" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AE41" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AF41" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AG41" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AH41" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -7996,64 +7962,64 @@
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
       <c r="R42" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T42" s="11" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
       <c r="U42" s="13"/>
       <c r="V42" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>#NUM!</v>
       </c>
       <c r="W42" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="X42" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="Y42" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="Z42" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AA42" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AB42" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AC42" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AD42" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AE42" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AF42" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AG42" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AH42" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -8077,64 +8043,64 @@
       <c r="O43" s="4"/>
       <c r="P43" s="4"/>
       <c r="R43" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T43" s="11" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
       <c r="U43" s="13"/>
       <c r="V43" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>#NUM!</v>
       </c>
       <c r="W43" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="X43" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="Y43" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="Z43" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AA43" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AB43" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AC43" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AD43" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AE43" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AF43" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AG43" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AH43" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -8158,60 +8124,60 @@
       <c r="O44" s="4"/>
       <c r="P44" s="4"/>
       <c r="R44" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T44" s="11" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
       <c r="U44" s="13"/>
       <c r="V44" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>#NUM!</v>
       </c>
       <c r="W44" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="X44" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="Y44" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="Z44" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AA44" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AB44" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AC44" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AD44" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AE44" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AF44" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AG44" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
       <c r="AH44" t="e">
@@ -8298,51 +8264,51 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F48" s="4">
-        <f t="shared" ref="F48:P55" si="20">1/24</f>
+        <f t="shared" ref="F48:P51" si="18">1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G48" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H48" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I48" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J48" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K48" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L48" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M48" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N48" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O48" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P48" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R48" s="3">
-        <f t="shared" ref="R48:R55" si="21">SUM(D48:P48)</f>
+        <f t="shared" ref="R48:R55" si="19">SUM(D48:P48)</f>
         <v>0.99999999999999956</v>
       </c>
       <c r="T48" s="11">
@@ -8355,51 +8321,51 @@
         <v>0</v>
       </c>
       <c r="W48">
-        <f t="shared" ref="W48:AH55" si="22">LOG(E48/E$3, 2)*E$57</f>
+        <f t="shared" ref="W48:AH55" si="20">LOG(E48/E$3, 2)*E$57</f>
         <v>0</v>
       </c>
       <c r="X48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Y48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Z48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AA48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AB48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AC48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AD48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AE48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AF48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AG48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AH48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -8413,112 +8379,112 @@
         <v>0.5</v>
       </c>
       <c r="E49" s="4">
-        <f t="shared" ref="E49:E55" si="23">1/24</f>
+        <f t="shared" ref="E49:E51" si="21">1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F49" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G49" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H49" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I49" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J49" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K49" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L49" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M49" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N49" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O49" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P49" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R49" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T49" s="11">
-        <f t="shared" ref="T49:T55" si="24">SUM(V49:AH49)</f>
+        <f t="shared" ref="T49:T55" si="22">SUM(V49:AH49)</f>
         <v>0</v>
       </c>
       <c r="U49" s="13"/>
       <c r="V49">
-        <f t="shared" ref="V49:V55" si="25">LOG(D49/D$3, 2)*D$57</f>
+        <f t="shared" ref="V49:V55" si="23">LOG(D49/D$3, 2)*D$57</f>
         <v>0</v>
       </c>
       <c r="W49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="X49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Y49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Z49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AA49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AB49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AC49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AD49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AE49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AF49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AG49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AH49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -8532,112 +8498,112 @@
         <v>0.5</v>
       </c>
       <c r="E50" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F50" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G50" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H50" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I50" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J50" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K50" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L50" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M50" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N50" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O50" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P50" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R50" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T50" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="U50" s="13"/>
       <c r="V50">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="W50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="X50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Y50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Z50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AA50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AB50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AC50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AD50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AE50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AF50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AG50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AH50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -8651,112 +8617,112 @@
         <v>0.5</v>
       </c>
       <c r="E51" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F51" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G51" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H51" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I51" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J51" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K51" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L51" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M51" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N51" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O51" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P51" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R51" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T51" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="U51" s="13"/>
       <c r="V51">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="W51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="X51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Y51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Z51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AA51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AB51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AC51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AD51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AE51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AF51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AG51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AH51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -8780,64 +8746,64 @@
       <c r="O52" s="4"/>
       <c r="P52" s="4"/>
       <c r="R52" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="T52" s="11" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>#NUM!</v>
       </c>
       <c r="U52" s="13"/>
       <c r="V52" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>#NUM!</v>
       </c>
       <c r="W52" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="X52" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="Y52" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="Z52" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AA52" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AB52" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AC52" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AD52" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AE52" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AF52" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AG52" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AH52" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -8861,64 +8827,64 @@
       <c r="O53" s="4"/>
       <c r="P53" s="4"/>
       <c r="R53" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="T53" s="11" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>#NUM!</v>
       </c>
       <c r="U53" s="13"/>
       <c r="V53" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>#NUM!</v>
       </c>
       <c r="W53" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="X53" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="Y53" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="Z53" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AA53" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AB53" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AC53" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AD53" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AE53" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AF53" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AG53" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AH53" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -8942,64 +8908,64 @@
       <c r="O54" s="4"/>
       <c r="P54" s="4"/>
       <c r="R54" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="T54" s="11" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>#NUM!</v>
       </c>
       <c r="U54" s="13"/>
       <c r="V54" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>#NUM!</v>
       </c>
       <c r="W54" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="X54" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="Y54" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="Z54" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AA54" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AB54" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AC54" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AD54" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AE54" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AF54" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AG54" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AH54" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -9023,64 +8989,64 @@
       <c r="O55" s="4"/>
       <c r="P55" s="4"/>
       <c r="R55" s="3">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="T55" s="11" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>#NUM!</v>
       </c>
       <c r="U55" s="13"/>
       <c r="V55" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>#NUM!</v>
       </c>
       <c r="W55" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="X55" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="Y55" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="Z55" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AA55" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AB55" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AC55" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AD55" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AE55" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AF55" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AG55" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
       <c r="AH55" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>#NUM!</v>
       </c>
     </row>

</xml_diff>